<commit_message>
last bit of transferring repo to mrc-ide
1. moved all of the drafts into the drafts/ folder
2. added and updated some small reference dataframes for diagnostics
3. moved written out parameter setting functions to main R folder from personal repo

to be done;
- details, sources, documentation on the parameters
- test writing for the parameter functions
</commit_message>
<xml_diff>
--- a/data-raw/who_summary_data.xlsx
+++ b/data-raw/who_summary_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icg20\Documents\GitHub\esft\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698BAA12-6C4E-4095-94E5-621CE690ECA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F991000-C6AC-4A33-AFA6-0E5F24388A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1470" windowWidth="21435" windowHeight="14730" firstSheet="4" activeTab="6" xr2:uid="{9304606A-D012-43B8-8D06-19B6C0873BB8}"/>
+    <workbookView xWindow="10920" yWindow="6105" windowWidth="14160" windowHeight="8880" firstSheet="5" activeTab="8" xr2:uid="{9304606A-D012-43B8-8D06-19B6C0873BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="wb_beds" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,15 @@
     <sheet name="population" sheetId="10" r:id="rId5"/>
     <sheet name="hwfe" sheetId="6" r:id="rId6"/>
     <sheet name="equipment" sheetId="5" r:id="rId7"/>
-    <sheet name="bed_nr_proxy" sheetId="2" r:id="rId8"/>
-    <sheet name="bed_perc_crit_proxy" sheetId="3" r:id="rId9"/>
-    <sheet name="transmission_scenarios" sheetId="9" r:id="rId10"/>
+    <sheet name="hours_per_shift" sheetId="11" r:id="rId8"/>
+    <sheet name="capacity_perc" sheetId="12" r:id="rId9"/>
+    <sheet name="bed_nr_proxy" sheetId="2" r:id="rId10"/>
+    <sheet name="bed_perc_crit_proxy" sheetId="3" r:id="rId11"/>
+    <sheet name="transmission_scenarios" sheetId="9" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
     <definedName name="Max_critical_capped_beds">'[1]Weekly Summary'!$BH$65</definedName>
@@ -127,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5533" uniqueCount="1208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5541" uniqueCount="1216">
   <si>
     <t>Country Name</t>
   </si>
@@ -3806,6 +3808,30 @@
   </si>
   <si>
     <t>amount_per_inpatient_sev_crit_patient_per_day</t>
+  </si>
+  <si>
+    <t>shifts</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>fully dedicated</t>
+  </si>
+  <si>
+    <t>primarily COVID</t>
+  </si>
+  <si>
+    <t>split evenly</t>
+  </si>
+  <si>
+    <t>limited capacity</t>
   </si>
 </sst>
 </file>
@@ -25426,6 +25452,169 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4553180F-2194-415F-B5E8-8D373957166B}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B1" t="s">
+        <v>683</v>
+      </c>
+      <c r="C1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5">
+        <v>4.82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3.41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2.08</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1.24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2.7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA7ED53-1E72-46A7-81C5-9784731B0538}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="A1:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B1" t="s">
+        <v>685</v>
+      </c>
+      <c r="C1" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6">
+        <v>3.5700000000000003E-2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6">
+        <v>3.32E-2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="6">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="6">
+        <f>AVERAGE(B2:B5)</f>
+        <v>2.725E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E553030B-655F-AE47-91AC-6146F1BB8A61}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -60609,7 +60798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA42A7E3-5F11-43A3-85DC-A6018F57571E}">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -62232,79 +62421,45 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4553180F-2194-415F-B5E8-8D373957166B}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135EF0CA-23E3-4624-9A64-0045304F68DF}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>564</v>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1208</v>
       </c>
       <c r="B1" t="s">
-        <v>683</v>
-      </c>
-      <c r="C1" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5">
-        <v>4.82</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="5">
-        <v>3.41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2.08</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1.24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -62313,80 +62468,53 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA7ED53-1E72-46A7-81C5-9784731B0538}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFFB039-61B1-4CA0-916C-A8C8D95740C6}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="A1:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>564</v>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1210</v>
       </c>
       <c r="B1" t="s">
-        <v>685</v>
-      </c>
-      <c r="C1" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="6">
-        <v>3.5700000000000003E-2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>1212</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="6">
-        <v>3.32E-2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>1213</v>
+      </c>
+      <c r="B3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="6">
-        <v>2.3800000000000002E-2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>1214</v>
+      </c>
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="6">
-        <v>1.6299999999999999E-2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="6">
-        <f>AVERAGE(B2:B5)</f>
-        <v>2.725E-2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
+        <v>1215</v>
+      </c>
+      <c r="B5">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>